<commit_message>
Multi-finemap and results for 78 PD-GWAS loci
</commit_message>
<xml_diff>
--- a/Data/GWAS/Nalls23andMe_2019/Nalls2019_TableS2.xlsx
+++ b/Data/GWAS/Nalls23andMe_2019/Nalls2019_TableS2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Fine_Mapping/Data/Parkinsons/Nalls_23andMe/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Fine_Mapping/Data/GWAS/Nalls23andMe_2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0276DF86-0D1C-214D-9DFE-5138726384A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423F7B54-553D-9B47-82E0-8EF4A6B0F91F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7440" yWindow="460" windowWidth="21360" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="254">
   <si>
     <t>SNP</t>
   </si>
@@ -782,12 +782,6 @@
   </si>
   <si>
     <t>DDRGK1</t>
-  </si>
-  <si>
-    <t>LRRK2_alt</t>
-  </si>
-  <si>
-    <t>LRRK2_rare</t>
   </si>
 </sst>
 </file>
@@ -1218,8 +1212,8 @@
   </sheetPr>
   <dimension ref="A1:AE983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7475,7 +7469,7 @@
         <v>40734202</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>255</v>
+        <v>158</v>
       </c>
       <c r="E67" s="17" t="s">
         <v>158</v>
@@ -7570,7 +7564,7 @@
         <v>40922572</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>254</v>
+        <v>158</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1" t="s">

</xml_diff>

<commit_message>
Push coloc changes to Minerva
</commit_message>
<xml_diff>
--- a/Data/GWAS/Nalls23andMe_2019/Nalls2019_TableS2.xlsx
+++ b/Data/GWAS/Nalls23andMe_2019/Nalls2019_TableS2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Fine_Mapping/Data/GWAS/Nalls23andMe_2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423F7B54-553D-9B47-82E0-8EF4A6B0F91F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74B027A-DFB4-E54D-9651-942F9D966CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="460" windowWidth="21360" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3680" yWindow="460" windowWidth="21360" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tableS2.tab" sheetId="1" r:id="rId1"/>
@@ -818,7 +818,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -837,6 +837,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7E79"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -850,7 +856,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -876,6 +882,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,6 +902,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF7E79"/>
       <color rgb="FF7A81FF"/>
     </mruColors>
   </colors>
@@ -1212,8 +1220,8 @@
   </sheetPr>
   <dimension ref="A1:AE983"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9827,7 +9835,7 @@
       <c r="C92" s="7">
         <v>43417273</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D92" s="17" t="s">
         <v>244</v>
       </c>
       <c r="E92" s="1"/>
@@ -9920,7 +9928,7 @@
       <c r="C93" s="7">
         <v>43744203</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D93" s="19" t="s">
         <v>204</v>
       </c>
       <c r="E93" s="12" t="s">
@@ -10015,7 +10023,7 @@
       <c r="C94" s="7">
         <v>43784228</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D94" s="19" t="s">
         <v>204</v>
       </c>
       <c r="E94" s="1"/>
@@ -10108,7 +10116,7 @@
       <c r="C95" s="7">
         <v>43798308</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D95" s="19" t="s">
         <v>204</v>
       </c>
       <c r="E95" s="12" t="s">
@@ -10203,7 +10211,7 @@
       <c r="C96" s="7">
         <v>43933307</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="D96" s="19" t="s">
         <v>247</v>
       </c>
       <c r="E96" s="1"/>
@@ -10296,7 +10304,7 @@
       <c r="C97" s="7">
         <v>44189067</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D97" s="19" t="s">
         <v>249</v>
       </c>
       <c r="E97" s="1"/>
@@ -10389,7 +10397,7 @@
       <c r="C98" s="7">
         <v>44800946</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="D98" s="19" t="s">
         <v>251</v>
       </c>
       <c r="E98" s="1"/>
@@ -10482,7 +10490,7 @@
       <c r="C99" s="7">
         <v>44866805</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D99" s="19" t="s">
         <v>205</v>
       </c>
       <c r="E99" s="1" t="s">

</xml_diff>

<commit_message>
Update scripts before IMPACT analysis
</commit_message>
<xml_diff>
--- a/Data/GWAS/Nalls23andMe_2019/Nalls2019_TableS2.xlsx
+++ b/Data/GWAS/Nalls23andMe_2019/Nalls2019_TableS2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Desktop/Fine_Mapping/Data/GWAS/Nalls23andMe_2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74B027A-DFB4-E54D-9651-942F9D966CB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F304339F-5A59-C042-9A8B-77D375309ABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3680" yWindow="460" windowWidth="21360" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1221,7 +1221,7 @@
   <dimension ref="A1:AE983"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9550,7 +9550,7 @@
       <c r="C89" s="7">
         <v>40741013</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D89" s="19" t="s">
         <v>197</v>
       </c>
       <c r="E89" s="1" t="s">
@@ -9645,7 +9645,7 @@
       <c r="C90" s="7">
         <v>42294337</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D90" s="19" t="s">
         <v>199</v>
       </c>
       <c r="E90" s="1" t="s">
@@ -9740,7 +9740,7 @@
       <c r="C91" s="7">
         <v>42434630</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D91" s="19" t="s">
         <v>201</v>
       </c>
       <c r="E91" s="1" t="s">
@@ -9835,7 +9835,7 @@
       <c r="C92" s="7">
         <v>43417273</v>
       </c>
-      <c r="D92" s="17" t="s">
+      <c r="D92" s="19" t="s">
         <v>244</v>
       </c>
       <c r="E92" s="1"/>

</xml_diff>